<commit_message>
Run from position registry deployment
</commit_message>
<xml_diff>
--- a/backend/checkpoints/polygon-USDC-EMXN-13.xlsx
+++ b/backend/checkpoints/polygon-USDC-EMXN-13.xlsx
@@ -450,7 +450,7 @@
         <v>Start Block</v>
       </c>
       <c r="B6" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -539,10 +539,10 @@
         <v>108422855638</v>
       </c>
       <c r="F2" t="str">
-        <v>0.003184</v>
+        <v>1.127882</v>
       </c>
       <c r="G2" t="str">
-        <v>0.041075</v>
+        <v>21.501656</v>
       </c>
     </row>
     <row r="3">
@@ -562,10 +562,10 @@
         <v>1082470260859</v>
       </c>
       <c r="F3" t="str">
-        <v>0.031788</v>
+        <v>11.260531</v>
       </c>
       <c r="G3" t="str">
-        <v>0.410092</v>
+        <v>214.667876</v>
       </c>
     </row>
     <row r="4">
@@ -585,10 +585,10 @@
         <v>1013587395</v>
       </c>
       <c r="F4" t="str">
-        <v>0.000029</v>
+        <v>0.010543</v>
       </c>
       <c r="G4" t="str">
-        <v>0.000383</v>
+        <v>0.201007</v>
       </c>
     </row>
     <row r="5">
@@ -611,7 +611,7 @@
         <v>0.061708</v>
       </c>
       <c r="G5" t="str">
-        <v>0</v>
+        <v>0.315928</v>
       </c>
     </row>
     <row r="6">
@@ -634,7 +634,7 @@
         <v>0.140217</v>
       </c>
       <c r="G6" t="str">
-        <v>1.808881</v>
+        <v>7.617206</v>
       </c>
     </row>
     <row r="7">
@@ -657,7 +657,7 @@
         <v>0.16358</v>
       </c>
       <c r="G7" t="str">
-        <v>2.11027</v>
+        <v>2.98331</v>
       </c>
     </row>
     <row r="8">
@@ -680,7 +680,7 @@
         <v>0.445789</v>
       </c>
       <c r="G8" t="str">
-        <v>2.806909</v>
+        <v>5.186691</v>
       </c>
     </row>
     <row r="9">
@@ -703,7 +703,7 @@
         <v>0.436283</v>
       </c>
       <c r="G9" t="str">
-        <v>0</v>
+        <v>2.233628</v>
       </c>
     </row>
     <row r="10">
@@ -726,180 +726,479 @@
         <v>0.840117</v>
       </c>
       <c r="G10" t="str">
-        <v>0</v>
+        <v>4.301126</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>56041</v>
+        <v>54620</v>
       </c>
       <c r="B11" t="str">
-        <v>0x40f81795f44b96BF88E16E055f2283B9cAEd9466</v>
+        <v>0xc1612C97537c2CC62a11FC4516367AB6F62d4B23</v>
       </c>
       <c r="C11">
-        <v>29140</v>
+        <v>-887270</v>
       </c>
       <c r="D11">
-        <v>29220</v>
+        <v>887270</v>
       </c>
       <c r="E11" t="str">
-        <v>2063978504756</v>
+        <v>687387</v>
       </c>
       <c r="F11" t="str">
-        <v>0.060612</v>
+        <v>0.000007</v>
       </c>
       <c r="G11" t="str">
-        <v>0.705219</v>
+        <v>0.000136</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>56048</v>
+        <v>54659</v>
       </c>
       <c r="B12" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
       </c>
       <c r="C12">
-        <v>29140</v>
+        <v>29010</v>
       </c>
       <c r="D12">
-        <v>29230</v>
+        <v>29250</v>
       </c>
       <c r="E12" t="str">
-        <v>3300151151331</v>
+        <v>430427826312</v>
       </c>
       <c r="F12" t="str">
-        <v>0.096915</v>
+        <v>4.477578</v>
       </c>
       <c r="G12" t="str">
-        <v>0.649495</v>
+        <v>85.359413</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>56049</v>
+        <v>54849</v>
       </c>
       <c r="B13" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
       <c r="C13">
-        <v>29090</v>
+        <v>-887270</v>
       </c>
       <c r="D13">
-        <v>29240</v>
+        <v>887270</v>
       </c>
       <c r="E13" t="str">
-        <v>3193100078685</v>
+        <v>41524</v>
       </c>
       <c r="F13" t="str">
-        <v>0.093771</v>
+        <v>0</v>
       </c>
       <c r="G13" t="str">
-        <v>0.467826</v>
+        <v>0.000008</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>56058</v>
+        <v>54863</v>
       </c>
       <c r="B14" t="str">
-        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
       <c r="C14">
-        <v>29170</v>
+        <v>-887270</v>
       </c>
       <c r="D14">
-        <v>29210</v>
+        <v>887270</v>
       </c>
       <c r="E14" t="str">
-        <v>50656195581128</v>
+        <v>737</v>
       </c>
       <c r="F14" t="str">
-        <v>1.487616</v>
+        <v>0</v>
       </c>
       <c r="G14" t="str">
-        <v>7.616106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>56142</v>
+        <v>54870</v>
       </c>
       <c r="B15" t="str">
-        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
       <c r="C15">
-        <v>29160</v>
+        <v>-887270</v>
       </c>
       <c r="D15">
-        <v>29220</v>
+        <v>887270</v>
       </c>
       <c r="E15" t="str">
-        <v>33597318063041</v>
+        <v>1306314</v>
       </c>
       <c r="F15" t="str">
-        <v>0.986649</v>
+        <v>0.000013</v>
       </c>
       <c r="G15" t="str">
-        <v>5.051322</v>
+        <v>0.000259</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>55869</v>
+        <v>54988</v>
       </c>
       <c r="B16" t="str">
-        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
       </c>
       <c r="C16">
-        <v>29130</v>
+        <v>-887270</v>
       </c>
       <c r="D16">
-        <v>29250</v>
+        <v>887270</v>
       </c>
       <c r="E16" t="str">
-        <v>0</v>
+        <v>2146804618</v>
       </c>
       <c r="F16" t="str">
-        <v>0</v>
+        <v>0.018012</v>
       </c>
       <c r="G16" t="str">
-        <v>0</v>
+        <v>0.34321</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
+        <v>55000</v>
+      </c>
+      <c r="B17" t="str">
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
+      </c>
+      <c r="C17">
+        <v>28910</v>
+      </c>
+      <c r="D17">
+        <v>29450</v>
+      </c>
+      <c r="E17" t="str">
+        <v>8500028065939</v>
+      </c>
+      <c r="F17" t="str">
+        <v>13.995462</v>
+      </c>
+      <c r="G17" t="str">
+        <v>293.550725</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>55680</v>
+      </c>
+      <c r="B18" t="str">
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
+      </c>
+      <c r="C18">
+        <v>29070</v>
+      </c>
+      <c r="D18">
+        <v>29270</v>
+      </c>
+      <c r="E18" t="str">
+        <v>34404015540441</v>
+      </c>
+      <c r="F18" t="str">
+        <v>1.010339</v>
+      </c>
+      <c r="G18" t="str">
+        <v>70.91594</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>55682</v>
+      </c>
+      <c r="B19" t="str">
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
+      </c>
+      <c r="C19">
+        <v>29110</v>
+      </c>
+      <c r="D19">
+        <v>29240</v>
+      </c>
+      <c r="E19" t="str">
+        <v>14957772702669</v>
+      </c>
+      <c r="F19" t="str">
+        <v>0.439263</v>
+      </c>
+      <c r="G19" t="str">
+        <v>23.86266</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>55723</v>
+      </c>
+      <c r="B20" t="str">
+        <v>0x93Cf0a22a26895650A8AaE960Bf85a01ec6A551C</v>
+      </c>
+      <c r="C20">
+        <v>29120</v>
+      </c>
+      <c r="D20">
+        <v>29210</v>
+      </c>
+      <c r="E20" t="str">
+        <v>9863753810772</v>
+      </c>
+      <c r="F20" t="str">
+        <v>0.289668</v>
+      </c>
+      <c r="G20" t="str">
+        <v>14.924372</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>55864</v>
+      </c>
+      <c r="B21" t="str">
+        <v>0xa614A83132a2e7368aDa71dA9331817c33706770</v>
+      </c>
+      <c r="C21">
+        <v>29010</v>
+      </c>
+      <c r="D21">
+        <v>29250</v>
+      </c>
+      <c r="E21" t="str">
+        <v>213394148753</v>
+      </c>
+      <c r="F21" t="str">
+        <v>0.006266</v>
+      </c>
+      <c r="G21" t="str">
+        <v>0.114298</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>55869</v>
+      </c>
+      <c r="B22" t="str">
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+      </c>
+      <c r="C22">
+        <v>29130</v>
+      </c>
+      <c r="D22">
+        <v>29250</v>
+      </c>
+      <c r="E22" t="str">
+        <v>0</v>
+      </c>
+      <c r="F22" t="str">
+        <v>0</v>
+      </c>
+      <c r="G22" t="str">
+        <v>5.627996</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>55913</v>
+      </c>
+      <c r="B23" t="str">
+        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+      <c r="C23">
+        <v>29120</v>
+      </c>
+      <c r="D23">
+        <v>29210</v>
+      </c>
+      <c r="E23" t="str">
+        <v>0</v>
+      </c>
+      <c r="F23" t="str">
+        <v>0</v>
+      </c>
+      <c r="G23" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
         <v>55914</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B24" t="str">
         <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
       </c>
-      <c r="C17">
+      <c r="C24">
         <v>29170</v>
       </c>
-      <c r="D17">
+      <c r="D24">
         <v>29200</v>
       </c>
-      <c r="E17" t="str">
+      <c r="E24" t="str">
         <v>19141817289270</v>
       </c>
-      <c r="F17" t="str">
+      <c r="F24" t="str">
         <v>0.562136</v>
       </c>
-      <c r="G17" t="str">
-        <v>0</v>
+      <c r="G24" t="str">
+        <v>7.810697</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>55934</v>
+      </c>
+      <c r="B25" t="str">
+        <v>0xE00E509c1968b4D586102a79Fabe9dcefEfb07f9</v>
+      </c>
+      <c r="C25">
+        <v>28570</v>
+      </c>
+      <c r="D25">
+        <v>29960</v>
+      </c>
+      <c r="E25" t="str">
+        <v>52692079948</v>
+      </c>
+      <c r="F25" t="str">
+        <v>0.001547</v>
+      </c>
+      <c r="G25" t="str">
+        <v>0.019962</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>56041</v>
+      </c>
+      <c r="B26" t="str">
+        <v>0x40f81795f44b96BF88E16E055f2283B9cAEd9466</v>
+      </c>
+      <c r="C26">
+        <v>29140</v>
+      </c>
+      <c r="D26">
+        <v>29220</v>
+      </c>
+      <c r="E26" t="str">
+        <v>2063978504756</v>
+      </c>
+      <c r="F26" t="str">
+        <v>0.060612</v>
+      </c>
+      <c r="G26" t="str">
+        <v>0.705219</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>56048</v>
+      </c>
+      <c r="B27" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+      <c r="C27">
+        <v>29140</v>
+      </c>
+      <c r="D27">
+        <v>29230</v>
+      </c>
+      <c r="E27" t="str">
+        <v>3300151151331</v>
+      </c>
+      <c r="F27" t="str">
+        <v>0.096915</v>
+      </c>
+      <c r="G27" t="str">
+        <v>0.649495</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>56049</v>
+      </c>
+      <c r="B28" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+      <c r="C28">
+        <v>29090</v>
+      </c>
+      <c r="D28">
+        <v>29240</v>
+      </c>
+      <c r="E28" t="str">
+        <v>3193100078685</v>
+      </c>
+      <c r="F28" t="str">
+        <v>0.093771</v>
+      </c>
+      <c r="G28" t="str">
+        <v>0.467826</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>56058</v>
+      </c>
+      <c r="B29" t="str">
+        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+      </c>
+      <c r="C29">
+        <v>29170</v>
+      </c>
+      <c r="D29">
+        <v>29210</v>
+      </c>
+      <c r="E29" t="str">
+        <v>50656195581128</v>
+      </c>
+      <c r="F29" t="str">
+        <v>1.487616</v>
+      </c>
+      <c r="G29" t="str">
+        <v>7.616106</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>56142</v>
+      </c>
+      <c r="B30" t="str">
+        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+      </c>
+      <c r="C30">
+        <v>29160</v>
+      </c>
+      <c r="D30">
+        <v>29220</v>
+      </c>
+      <c r="E30" t="str">
+        <v>33597318063041</v>
+      </c>
+      <c r="F30" t="str">
+        <v>0.986649</v>
+      </c>
+      <c r="G30" t="str">
+        <v>5.051322</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G17"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G30"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -923,7 +1222,7 @@
         <v>39240</v>
       </c>
       <c r="B2" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C2" t="str">
         <v>108422855638</v>
@@ -951,7 +1250,7 @@
         <v>40441</v>
       </c>
       <c r="B4" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C4" t="str">
         <v>1082470260859</v>
@@ -979,7 +1278,7 @@
         <v>43508</v>
       </c>
       <c r="B6" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C6" t="str">
         <v>1013587395</v>
@@ -1007,7 +1306,7 @@
         <v>48604</v>
       </c>
       <c r="B8" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C8" t="str">
         <v>2101301186666</v>
@@ -1035,7 +1334,7 @@
         <v>52989</v>
       </c>
       <c r="B10" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C10" t="str">
         <v>4774674820800</v>
@@ -1063,7 +1362,7 @@
         <v>55716</v>
       </c>
       <c r="B12" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C12" t="str">
         <v>5570213347780</v>
@@ -1091,7 +1390,7 @@
         <v>55817</v>
       </c>
       <c r="B14" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C14" t="str">
         <v>15179979571372</v>
@@ -1119,7 +1418,7 @@
         <v>55819</v>
       </c>
       <c r="B16" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C16" t="str">
         <v>14856293253341</v>
@@ -1147,7 +1446,7 @@
         <v>55822</v>
       </c>
       <c r="B18" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C18" t="str">
         <v>28607620072666</v>
@@ -1172,10 +1471,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>56041</v>
+        <v>54620</v>
       </c>
       <c r="B20" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C20" t="str">
         <v>0</v>
@@ -1186,248 +1485,248 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>56041</v>
+        <v>54620</v>
       </c>
       <c r="B21" t="str">
-        <v>78611428</v>
+        <v>78380505</v>
       </c>
       <c r="C21" t="str">
-        <v>2063978504756</v>
+        <v>687387</v>
       </c>
       <c r="D21" t="str">
-        <v>0x40f81795f44b96BF88E16E055f2283B9cAEd9466</v>
+        <v>0xc1612C97537c2CC62a11FC4516367AB6F62d4B23</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>56041</v>
+        <v>54620</v>
       </c>
       <c r="B22" t="str">
-        <v>78611449</v>
+        <v>78900356</v>
       </c>
       <c r="C22" t="str">
-        <v>2063978504756</v>
+        <v>687387</v>
       </c>
       <c r="D22" t="str">
-        <v>0x40f81795f44b96BF88E16E055f2283B9cAEd9466</v>
+        <v>0xc1612C97537c2CC62a11FC4516367AB6F62d4B23</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>56041</v>
+        <v>54659</v>
       </c>
       <c r="B23" t="str">
-        <v>78900356</v>
+        <v>78331507</v>
       </c>
       <c r="C23" t="str">
-        <v>2063978504756</v>
+        <v>0</v>
       </c>
       <c r="D23" t="str">
-        <v>0x40f81795f44b96BF88E16E055f2283B9cAEd9466</v>
+        <v>0x0000000000000000000000000000000000000000</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>56048</v>
+        <v>54659</v>
       </c>
       <c r="B24" t="str">
-        <v>78597968</v>
+        <v>78384958</v>
       </c>
       <c r="C24" t="str">
-        <v>0</v>
+        <v>430427826312</v>
       </c>
       <c r="D24" t="str">
-        <v>0x0000000000000000000000000000000000000000</v>
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>56048</v>
+        <v>54659</v>
       </c>
       <c r="B25" t="str">
-        <v>78613594</v>
+        <v>78546368</v>
       </c>
       <c r="C25" t="str">
-        <v>2865967464325</v>
+        <v>430427826312</v>
       </c>
       <c r="D25" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>56048</v>
+        <v>54659</v>
       </c>
       <c r="B26" t="str">
-        <v>78613650</v>
+        <v>78900356</v>
       </c>
       <c r="C26" t="str">
-        <v>2865967464325</v>
+        <v>430427826312</v>
       </c>
       <c r="D26" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>56048</v>
+        <v>54849</v>
       </c>
       <c r="B27" t="str">
-        <v>78719872</v>
+        <v>78331507</v>
       </c>
       <c r="C27" t="str">
-        <v>3300151151331</v>
+        <v>0</v>
       </c>
       <c r="D27" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0x0000000000000000000000000000000000000000</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>56048</v>
+        <v>54849</v>
       </c>
       <c r="B28" t="str">
-        <v>78900356</v>
+        <v>78413557</v>
       </c>
       <c r="C28" t="str">
-        <v>3300151151331</v>
+        <v>41524</v>
       </c>
       <c r="D28" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>56049</v>
+        <v>54849</v>
       </c>
       <c r="B29" t="str">
-        <v>78597968</v>
+        <v>78900356</v>
       </c>
       <c r="C29" t="str">
-        <v>0</v>
+        <v>41524</v>
       </c>
       <c r="D29" t="str">
-        <v>0x0000000000000000000000000000000000000000</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>56049</v>
+        <v>54863</v>
       </c>
       <c r="B30" t="str">
-        <v>78613890</v>
+        <v>78331507</v>
       </c>
       <c r="C30" t="str">
-        <v>3110928445275</v>
+        <v>0</v>
       </c>
       <c r="D30" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0x0000000000000000000000000000000000000000</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>56049</v>
+        <v>54863</v>
       </c>
       <c r="B31" t="str">
-        <v>78613917</v>
+        <v>78414928</v>
       </c>
       <c r="C31" t="str">
-        <v>3110928445275</v>
+        <v>737</v>
       </c>
       <c r="D31" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>56049</v>
+        <v>54863</v>
       </c>
       <c r="B32" t="str">
-        <v>78719935</v>
+        <v>78900356</v>
       </c>
       <c r="C32" t="str">
-        <v>3193100078685</v>
+        <v>737</v>
       </c>
       <c r="D32" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>56049</v>
+        <v>54870</v>
       </c>
       <c r="B33" t="str">
-        <v>78900356</v>
+        <v>78331507</v>
       </c>
       <c r="C33" t="str">
-        <v>3193100078685</v>
+        <v>0</v>
       </c>
       <c r="D33" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0x0000000000000000000000000000000000000000</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>56058</v>
+        <v>54870</v>
       </c>
       <c r="B34" t="str">
-        <v>78597968</v>
+        <v>78415454</v>
       </c>
       <c r="C34" t="str">
-        <v>0</v>
+        <v>7384</v>
       </c>
       <c r="D34" t="str">
-        <v>0x0000000000000000000000000000000000000000</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>56058</v>
+        <v>54870</v>
       </c>
       <c r="B35" t="str">
-        <v>78615146</v>
+        <v>78416424</v>
       </c>
       <c r="C35" t="str">
-        <v>50656195581128</v>
+        <v>190771</v>
       </c>
       <c r="D35" t="str">
-        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>56058</v>
+        <v>54870</v>
       </c>
       <c r="B36" t="str">
-        <v>78615306</v>
+        <v>78416671</v>
       </c>
       <c r="C36" t="str">
-        <v>50656195581128</v>
+        <v>1306314</v>
       </c>
       <c r="D36" t="str">
-        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>56058</v>
+        <v>54870</v>
       </c>
       <c r="B37" t="str">
         <v>78900356</v>
       </c>
       <c r="C37" t="str">
-        <v>50656195581128</v>
+        <v>1306314</v>
       </c>
       <c r="D37" t="str">
-        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+        <v>0x329e6cBdD16cAD2f51D97d2E8F09612f12D45A6d</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>56142</v>
+        <v>54988</v>
       </c>
       <c r="B38" t="str">
-        <v>78597968</v>
+        <v>78331507</v>
       </c>
       <c r="C38" t="str">
         <v>0</v>
@@ -1438,154 +1737,1050 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>56142</v>
+        <v>54988</v>
       </c>
       <c r="B39" t="str">
-        <v>78625356</v>
+        <v>78430534</v>
       </c>
       <c r="C39" t="str">
-        <v>33597318063041</v>
+        <v>2146804618</v>
       </c>
       <c r="D39" t="str">
-        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>56142</v>
+        <v>54988</v>
       </c>
       <c r="B40" t="str">
-        <v>78625381</v>
+        <v>78530279</v>
       </c>
       <c r="C40" t="str">
-        <v>33597318063041</v>
+        <v>2146804618</v>
       </c>
       <c r="D40" t="str">
-        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>56142</v>
+        <v>54988</v>
       </c>
       <c r="B41" t="str">
-        <v>78900356</v>
+        <v>78533370</v>
       </c>
       <c r="C41" t="str">
-        <v>33597318063041</v>
+        <v>2146804618</v>
       </c>
       <c r="D41" t="str">
-        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>55869</v>
+        <v>54988</v>
       </c>
       <c r="B42" t="str">
-        <v>78597968</v>
+        <v>78533479</v>
       </c>
       <c r="C42" t="str">
-        <v>0</v>
+        <v>2146804618</v>
       </c>
       <c r="D42" t="str">
-        <v>0x0000000000000000000000000000000000000000</v>
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>55869</v>
+        <v>54988</v>
       </c>
       <c r="B43" t="str">
-        <v>78716400</v>
+        <v>78900356</v>
       </c>
       <c r="C43" t="str">
-        <v>0</v>
+        <v>2146804618</v>
       </c>
       <c r="D43" t="str">
-        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>55869</v>
+        <v>55000</v>
       </c>
       <c r="B44" t="str">
-        <v>78900356</v>
+        <v>78331507</v>
       </c>
       <c r="C44" t="str">
         <v>0</v>
       </c>
       <c r="D44" t="str">
-        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+        <v>0x0000000000000000000000000000000000000000</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>55914</v>
+        <v>55000</v>
       </c>
       <c r="B45" t="str">
-        <v>78597968</v>
+        <v>78433054</v>
       </c>
       <c r="C45" t="str">
-        <v>0</v>
+        <v>8500028065939</v>
       </c>
       <c r="D45" t="str">
-        <v>0x0000000000000000000000000000000000000000</v>
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>55914</v>
+        <v>55000</v>
       </c>
       <c r="B46" t="str">
-        <v>78813544</v>
+        <v>78530290</v>
       </c>
       <c r="C46" t="str">
-        <v>18890063930711</v>
+        <v>8500028065939</v>
       </c>
       <c r="D46" t="str">
-        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>55914</v>
+        <v>55000</v>
       </c>
       <c r="B47" t="str">
-        <v>78813572</v>
+        <v>78533381</v>
       </c>
       <c r="C47" t="str">
-        <v>19141817289270</v>
+        <v>8500028065939</v>
       </c>
       <c r="D47" t="str">
-        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
+        <v>55000</v>
+      </c>
+      <c r="B48" t="str">
+        <v>78533445</v>
+      </c>
+      <c r="C48" t="str">
+        <v>8500028065939</v>
+      </c>
+      <c r="D48" t="str">
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>55000</v>
+      </c>
+      <c r="B49" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C49" t="str">
+        <v>8500028065939</v>
+      </c>
+      <c r="D49" t="str">
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>55680</v>
+      </c>
+      <c r="B50" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C50" t="str">
+        <v>0</v>
+      </c>
+      <c r="D50" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>55680</v>
+      </c>
+      <c r="B51" t="str">
+        <v>78558938</v>
+      </c>
+      <c r="C51" t="str">
+        <v>34404015540441</v>
+      </c>
+      <c r="D51" t="str">
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>55680</v>
+      </c>
+      <c r="B52" t="str">
+        <v>78559123</v>
+      </c>
+      <c r="C52" t="str">
+        <v>34404015540441</v>
+      </c>
+      <c r="D52" t="str">
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>55680</v>
+      </c>
+      <c r="B53" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C53" t="str">
+        <v>34404015540441</v>
+      </c>
+      <c r="D53" t="str">
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>55682</v>
+      </c>
+      <c r="B54" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C54" t="str">
+        <v>0</v>
+      </c>
+      <c r="D54" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>55682</v>
+      </c>
+      <c r="B55" t="str">
+        <v>78559089</v>
+      </c>
+      <c r="C55" t="str">
+        <v>14957772702669</v>
+      </c>
+      <c r="D55" t="str">
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>55682</v>
+      </c>
+      <c r="B56" t="str">
+        <v>78559132</v>
+      </c>
+      <c r="C56" t="str">
+        <v>14957772702669</v>
+      </c>
+      <c r="D56" t="str">
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>55682</v>
+      </c>
+      <c r="B57" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C57" t="str">
+        <v>14957772702669</v>
+      </c>
+      <c r="D57" t="str">
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>55723</v>
+      </c>
+      <c r="B58" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C58" t="str">
+        <v>0</v>
+      </c>
+      <c r="D58" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>55723</v>
+      </c>
+      <c r="B59" t="str">
+        <v>78568485</v>
+      </c>
+      <c r="C59" t="str">
+        <v>9863753810772</v>
+      </c>
+      <c r="D59" t="str">
+        <v>0x93Cf0a22a26895650A8AaE960Bf85a01ec6A551C</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>55723</v>
+      </c>
+      <c r="B60" t="str">
+        <v>78568518</v>
+      </c>
+      <c r="C60" t="str">
+        <v>9863753810772</v>
+      </c>
+      <c r="D60" t="str">
+        <v>0x93Cf0a22a26895650A8AaE960Bf85a01ec6A551C</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>55723</v>
+      </c>
+      <c r="B61" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C61" t="str">
+        <v>9863753810772</v>
+      </c>
+      <c r="D61" t="str">
+        <v>0x93Cf0a22a26895650A8AaE960Bf85a01ec6A551C</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>55864</v>
+      </c>
+      <c r="B62" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C62" t="str">
+        <v>0</v>
+      </c>
+      <c r="D62" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>55864</v>
+      </c>
+      <c r="B63" t="str">
+        <v>78587257</v>
+      </c>
+      <c r="C63" t="str">
+        <v>213394148753</v>
+      </c>
+      <c r="D63" t="str">
+        <v>0xa614A83132a2e7368aDa71dA9331817c33706770</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>55864</v>
+      </c>
+      <c r="B64" t="str">
+        <v>78587290</v>
+      </c>
+      <c r="C64" t="str">
+        <v>213394148753</v>
+      </c>
+      <c r="D64" t="str">
+        <v>0xa614A83132a2e7368aDa71dA9331817c33706770</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>55864</v>
+      </c>
+      <c r="B65" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C65" t="str">
+        <v>213394148753</v>
+      </c>
+      <c r="D65" t="str">
+        <v>0xa614A83132a2e7368aDa71dA9331817c33706770</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>55869</v>
+      </c>
+      <c r="B66" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C66" t="str">
+        <v>0</v>
+      </c>
+      <c r="D66" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>55869</v>
+      </c>
+      <c r="B67" t="str">
+        <v>78588023</v>
+      </c>
+      <c r="C67" t="str">
+        <v>4068410686307</v>
+      </c>
+      <c r="D67" t="str">
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>55869</v>
+      </c>
+      <c r="B68" t="str">
+        <v>78588574</v>
+      </c>
+      <c r="C68" t="str">
+        <v>4068410686307</v>
+      </c>
+      <c r="D68" t="str">
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>55869</v>
+      </c>
+      <c r="B69" t="str">
+        <v>78588825</v>
+      </c>
+      <c r="C69" t="str">
+        <v>4130024264263</v>
+      </c>
+      <c r="D69" t="str">
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>55869</v>
+      </c>
+      <c r="B70" t="str">
+        <v>78588866</v>
+      </c>
+      <c r="C70" t="str">
+        <v>4130024264263</v>
+      </c>
+      <c r="D70" t="str">
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>55869</v>
+      </c>
+      <c r="B71" t="str">
+        <v>78588903</v>
+      </c>
+      <c r="C71" t="str">
+        <v>4130024264263</v>
+      </c>
+      <c r="D71" t="str">
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>55869</v>
+      </c>
+      <c r="B72" t="str">
+        <v>78716400</v>
+      </c>
+      <c r="C72" t="str">
+        <v>4130024264263</v>
+      </c>
+      <c r="D72" t="str">
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>55869</v>
+      </c>
+      <c r="B73" t="str">
+        <v>78716400</v>
+      </c>
+      <c r="C73" t="str">
+        <v>0</v>
+      </c>
+      <c r="D73" t="str">
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>55869</v>
+      </c>
+      <c r="B74" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C74" t="str">
+        <v>0</v>
+      </c>
+      <c r="D74" t="str">
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>55913</v>
+      </c>
+      <c r="B75" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C75" t="str">
+        <v>0</v>
+      </c>
+      <c r="D75" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>55913</v>
+      </c>
+      <c r="B76" t="str">
+        <v>78594142</v>
+      </c>
+      <c r="C76" t="str">
+        <v>2380098461035</v>
+      </c>
+      <c r="D76" t="str">
+        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>55913</v>
+      </c>
+      <c r="B77" t="str">
+        <v>78594178</v>
+      </c>
+      <c r="C77" t="str">
+        <v>0</v>
+      </c>
+      <c r="D77" t="str">
+        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>55913</v>
+      </c>
+      <c r="B78" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C78" t="str">
+        <v>0</v>
+      </c>
+      <c r="D78" t="str">
+        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
         <v>55914</v>
       </c>
-      <c r="B48" t="str">
+      <c r="B79" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C79" t="str">
+        <v>0</v>
+      </c>
+      <c r="D79" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>55914</v>
+      </c>
+      <c r="B80" t="str">
+        <v>78594296</v>
+      </c>
+      <c r="C80" t="str">
+        <v>4174052211341</v>
+      </c>
+      <c r="D80" t="str">
+        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>55914</v>
+      </c>
+      <c r="B81" t="str">
+        <v>78594393</v>
+      </c>
+      <c r="C81" t="str">
+        <v>16852701766190</v>
+      </c>
+      <c r="D81" t="str">
+        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>55914</v>
+      </c>
+      <c r="B82" t="str">
+        <v>78594481</v>
+      </c>
+      <c r="C82" t="str">
+        <v>18890063930711</v>
+      </c>
+      <c r="D82" t="str">
+        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>55914</v>
+      </c>
+      <c r="B83" t="str">
+        <v>78594531</v>
+      </c>
+      <c r="C83" t="str">
+        <v>18890063930711</v>
+      </c>
+      <c r="D83" t="str">
+        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>55914</v>
+      </c>
+      <c r="B84" t="str">
+        <v>78813544</v>
+      </c>
+      <c r="C84" t="str">
+        <v>18890063930711</v>
+      </c>
+      <c r="D84" t="str">
+        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>55914</v>
+      </c>
+      <c r="B85" t="str">
+        <v>78813572</v>
+      </c>
+      <c r="C85" t="str">
+        <v>19141817289270</v>
+      </c>
+      <c r="D85" t="str">
+        <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>55914</v>
+      </c>
+      <c r="B86" t="str">
         <v>78900356</v>
       </c>
-      <c r="C48" t="str">
+      <c r="C86" t="str">
         <v>19141817289270</v>
       </c>
-      <c r="D48" t="str">
+      <c r="D86" t="str">
         <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>55934</v>
+      </c>
+      <c r="B87" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C87" t="str">
+        <v>0</v>
+      </c>
+      <c r="D87" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>55934</v>
+      </c>
+      <c r="B88" t="str">
+        <v>78596200</v>
+      </c>
+      <c r="C88" t="str">
+        <v>52692079948</v>
+      </c>
+      <c r="D88" t="str">
+        <v>0xE00E509c1968b4D586102a79Fabe9dcefEfb07f9</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>55934</v>
+      </c>
+      <c r="B89" t="str">
+        <v>78596301</v>
+      </c>
+      <c r="C89" t="str">
+        <v>52692079948</v>
+      </c>
+      <c r="D89" t="str">
+        <v>0xE00E509c1968b4D586102a79Fabe9dcefEfb07f9</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>55934</v>
+      </c>
+      <c r="B90" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C90" t="str">
+        <v>52692079948</v>
+      </c>
+      <c r="D90" t="str">
+        <v>0xE00E509c1968b4D586102a79Fabe9dcefEfb07f9</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>56041</v>
+      </c>
+      <c r="B91" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C91" t="str">
+        <v>0</v>
+      </c>
+      <c r="D91" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>56041</v>
+      </c>
+      <c r="B92" t="str">
+        <v>78611428</v>
+      </c>
+      <c r="C92" t="str">
+        <v>2063978504756</v>
+      </c>
+      <c r="D92" t="str">
+        <v>0x40f81795f44b96BF88E16E055f2283B9cAEd9466</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>56041</v>
+      </c>
+      <c r="B93" t="str">
+        <v>78611449</v>
+      </c>
+      <c r="C93" t="str">
+        <v>2063978504756</v>
+      </c>
+      <c r="D93" t="str">
+        <v>0x40f81795f44b96BF88E16E055f2283B9cAEd9466</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>56041</v>
+      </c>
+      <c r="B94" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C94" t="str">
+        <v>2063978504756</v>
+      </c>
+      <c r="D94" t="str">
+        <v>0x40f81795f44b96BF88E16E055f2283B9cAEd9466</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>56048</v>
+      </c>
+      <c r="B95" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C95" t="str">
+        <v>0</v>
+      </c>
+      <c r="D95" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>56048</v>
+      </c>
+      <c r="B96" t="str">
+        <v>78613594</v>
+      </c>
+      <c r="C96" t="str">
+        <v>2865967464325</v>
+      </c>
+      <c r="D96" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>56048</v>
+      </c>
+      <c r="B97" t="str">
+        <v>78613650</v>
+      </c>
+      <c r="C97" t="str">
+        <v>2865967464325</v>
+      </c>
+      <c r="D97" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>56048</v>
+      </c>
+      <c r="B98" t="str">
+        <v>78719872</v>
+      </c>
+      <c r="C98" t="str">
+        <v>3300151151331</v>
+      </c>
+      <c r="D98" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>56048</v>
+      </c>
+      <c r="B99" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C99" t="str">
+        <v>3300151151331</v>
+      </c>
+      <c r="D99" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>56049</v>
+      </c>
+      <c r="B100" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C100" t="str">
+        <v>0</v>
+      </c>
+      <c r="D100" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>56049</v>
+      </c>
+      <c r="B101" t="str">
+        <v>78613890</v>
+      </c>
+      <c r="C101" t="str">
+        <v>3110928445275</v>
+      </c>
+      <c r="D101" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>56049</v>
+      </c>
+      <c r="B102" t="str">
+        <v>78613917</v>
+      </c>
+      <c r="C102" t="str">
+        <v>3110928445275</v>
+      </c>
+      <c r="D102" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>56049</v>
+      </c>
+      <c r="B103" t="str">
+        <v>78719935</v>
+      </c>
+      <c r="C103" t="str">
+        <v>3193100078685</v>
+      </c>
+      <c r="D103" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>56049</v>
+      </c>
+      <c r="B104" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C104" t="str">
+        <v>3193100078685</v>
+      </c>
+      <c r="D104" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>56058</v>
+      </c>
+      <c r="B105" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C105" t="str">
+        <v>0</v>
+      </c>
+      <c r="D105" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>56058</v>
+      </c>
+      <c r="B106" t="str">
+        <v>78615146</v>
+      </c>
+      <c r="C106" t="str">
+        <v>50656195581128</v>
+      </c>
+      <c r="D106" t="str">
+        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>56058</v>
+      </c>
+      <c r="B107" t="str">
+        <v>78615306</v>
+      </c>
+      <c r="C107" t="str">
+        <v>50656195581128</v>
+      </c>
+      <c r="D107" t="str">
+        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>56058</v>
+      </c>
+      <c r="B108" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C108" t="str">
+        <v>50656195581128</v>
+      </c>
+      <c r="D108" t="str">
+        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>56142</v>
+      </c>
+      <c r="B109" t="str">
+        <v>78331507</v>
+      </c>
+      <c r="C109" t="str">
+        <v>0</v>
+      </c>
+      <c r="D109" t="str">
+        <v>0x0000000000000000000000000000000000000000</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>56142</v>
+      </c>
+      <c r="B110" t="str">
+        <v>78625356</v>
+      </c>
+      <c r="C110" t="str">
+        <v>33597318063041</v>
+      </c>
+      <c r="D110" t="str">
+        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>56142</v>
+      </c>
+      <c r="B111" t="str">
+        <v>78625381</v>
+      </c>
+      <c r="C111" t="str">
+        <v>33597318063041</v>
+      </c>
+      <c r="D111" t="str">
+        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>56142</v>
+      </c>
+      <c r="B112" t="str">
+        <v>78900356</v>
+      </c>
+      <c r="C112" t="str">
+        <v>33597318063041</v>
+      </c>
+      <c r="D112" t="str">
+        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D48"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D112"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1609,75 +2804,177 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>0x40f81795f44b96BF88E16E055f2283B9cAEd9466</v>
+        <v>0x0776b74e2dC3fe4f25FdAf18c0eBB274b574dba8</v>
       </c>
       <c r="B2" t="str">
-        <v>0.060612</v>
+        <v>1.462242</v>
       </c>
       <c r="C2" t="str">
-        <v>0.705219</v>
+        <v>79.635823</v>
       </c>
       <c r="D2" t="str">
-        <v>16772.93</v>
+        <v>277480.25</v>
       </c>
       <c r="E2" t="str">
-        <v>115277</v>
+        <v>5639586</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+        <v>0xE71A7e9866325995f1071e3C79e01595cf88bE30</v>
       </c>
       <c r="B3" t="str">
-        <v>0.190686</v>
+        <v>0.249682</v>
       </c>
       <c r="C3" t="str">
-        <v>1.117321</v>
+        <v>17.525271</v>
       </c>
       <c r="D3" t="str">
-        <v>40346.87</v>
+        <v>57516.43</v>
       </c>
       <c r="E3" t="str">
-        <v>277296</v>
+        <v>1168980</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+        <v>0x93Cf0a22a26895650A8AaE960Bf85a01ec6A551C</v>
       </c>
       <c r="B4" t="str">
-        <v>2.474265</v>
+        <v>0.289668</v>
       </c>
       <c r="C4" t="str">
-        <v>12.667428</v>
+        <v>14.924372</v>
       </c>
       <c r="D4" t="str">
-        <v>502880.19</v>
+        <v>52771.07</v>
       </c>
       <c r="E4" t="str">
-        <v>3456195</v>
+        <v>1072534</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
+        <v>0xa614A83132a2e7368aDa71dA9331817c33706770</v>
+      </c>
+      <c r="B5" t="str">
+        <v>0.006266</v>
+      </c>
+      <c r="C5" t="str">
+        <v>0.114298</v>
+      </c>
+      <c r="D5" t="str">
+        <v>603.26</v>
+      </c>
+      <c r="E5" t="str">
+        <v>12261</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>0x19D27Bd32c639C4b5DaA9b9D05AD2401A79224F0</v>
+      </c>
+      <c r="B6" t="str">
+        <v>0</v>
+      </c>
+      <c r="C6" t="str">
+        <v>0</v>
+      </c>
+      <c r="D6" t="str">
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
         <v>0xC35Bd8e35D5C866F90bD8Db563680712560A9765</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B7" t="str">
         <v>0.562136</v>
       </c>
-      <c r="C5" t="str">
-        <v>0</v>
-      </c>
-      <c r="D5" t="str">
-        <v>0</v>
-      </c>
-      <c r="E5" t="str">
-        <v>0</v>
+      <c r="C7" t="str">
+        <v>7.156483</v>
+      </c>
+      <c r="D7" t="str">
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>0xE00E509c1968b4D586102a79Fabe9dcefEfb07f9</v>
+      </c>
+      <c r="B8" t="str">
+        <v>0.001547</v>
+      </c>
+      <c r="C8" t="str">
+        <v>0.019962</v>
+      </c>
+      <c r="D8" t="str">
+        <v>127.63</v>
+      </c>
+      <c r="E8" t="str">
+        <v>2594</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>0x40f81795f44b96BF88E16E055f2283B9cAEd9466</v>
+      </c>
+      <c r="B9" t="str">
+        <v>0.060612</v>
+      </c>
+      <c r="C9" t="str">
+        <v>0.705219</v>
+      </c>
+      <c r="D9" t="str">
+        <v>4802.33</v>
+      </c>
+      <c r="E9" t="str">
+        <v>97604</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>0xa60209fbC5e75fBE99dAcEe53CD763850615fE10</v>
+      </c>
+      <c r="B10" t="str">
+        <v>0.190686</v>
+      </c>
+      <c r="C10" t="str">
+        <v>1.117321</v>
+      </c>
+      <c r="D10" t="str">
+        <v>12265.87</v>
+      </c>
+      <c r="E10" t="str">
+        <v>249295</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>0x8087d7785051A23Fb21cb2dc240A409351A9E0a8</v>
+      </c>
+      <c r="B11" t="str">
+        <v>2.474265</v>
+      </c>
+      <c r="C11" t="str">
+        <v>12.667428</v>
+      </c>
+      <c r="D11" t="str">
+        <v>154433.13</v>
+      </c>
+      <c r="E11" t="str">
+        <v>3138742</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>